<commit_message>
Updated with first case and death
</commit_message>
<xml_diff>
--- a/Government responses.xlsx
+++ b/Government responses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Howard\Documents\Bristol\Covid-19\Cost-effectiveness of lockdowns\Government responses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D38E306-7F85-464E-91FE-8755CBFB65B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3EA882-884B-48D1-8DE2-78AC1A16006B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13155" xr2:uid="{F24129F8-4FA3-43CF-BEA4-CC55ED639602}"/>
   </bookViews>
@@ -19,6 +19,7 @@
     <sheet name="Germany" sheetId="3" r:id="rId4"/>
     <sheet name="Ireland" sheetId="6" r:id="rId5"/>
     <sheet name="South Korea" sheetId="5" r:id="rId6"/>
+    <sheet name="Testing" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="133">
   <si>
     <t>First confirmed case</t>
   </si>
@@ -422,6 +423,21 @@
   </si>
   <si>
     <t>By this date 100,000 citations issued and 1000 people arrested for violating social disatncing. Fines range from 100 to 30,000 euro, with imprisonment up to 4 months. Drones used for enforcement.</t>
+  </si>
+  <si>
+    <t>Cases/million</t>
+  </si>
+  <si>
+    <t>Test/million</t>
+  </si>
+  <si>
+    <t>Ratio test/case</t>
+  </si>
+  <si>
+    <t>England and Wales (UK)</t>
+  </si>
+  <si>
+    <t>10th death</t>
   </si>
 </sst>
 </file>
@@ -474,11 +490,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -797,12 +814,13 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="3" width="10.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.796875" customWidth="1"/>
+    <col min="3" max="3" width="20.73046875" customWidth="1"/>
     <col min="8" max="8" width="106.53125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -814,6 +832,9 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1495,4 +1516,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{882AC3CF-4179-4B6F-9588-4CFC250D42E1}">
+  <dimension ref="A3:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D3:D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="4" max="4" width="14.86328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4">
+        <v>6366</v>
+      </c>
+      <c r="C4">
+        <v>116543</v>
+      </c>
+      <c r="D4" s="4">
+        <f>C4/B4</f>
+        <v>18.307100219918315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5">
+        <v>2359</v>
+      </c>
+      <c r="C5">
+        <v>70100</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" ref="D5:D8" si="0">C5/B5</f>
+        <v>29.715981348028826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>7071</v>
+      </c>
+      <c r="C6">
+        <v>51397</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>7.2687031537264888</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7">
+        <v>5169</v>
+      </c>
+      <c r="C7">
+        <v>94738</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>18.328109885857998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>4209</v>
+      </c>
+      <c r="C8">
+        <v>156889</v>
+      </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>37.274649560465669</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>